<commit_message>
Tratamento Dos Dados Excel
</commit_message>
<xml_diff>
--- a/ES/src/Long-Method.xlsx
+++ b/ES/src/Long-Method.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\Desktop\faculdade\4ano\ES\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{571A33B7-7BCB-41B5-99A1-1AE31E79082F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5F8878F6-68FB-45CB-9CB6-01264C425E76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="29070" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="long-method" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'long-method'!$A$1:$M$421</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -3758,8 +3754,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L421"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3772,7 +3768,7 @@
     <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
     <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>